<commit_message>
Add dictionary sanitization for sheet_items - Object.sanitize_sheet_items - Extend tests, better naming in tests - Update README.md - Bump version to 0.0.5
</commit_message>
<xml_diff>
--- a/tests/inventory.xlsx
+++ b/tests/inventory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomas/Downloads/sheet2dict/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomas/Dropbox/Python_Tools/sheet2dict/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D64EB86-F9E1-3E4F-B8BC-981B7A2A3D5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63881F2-756F-9B45-A42E-50346FD8A317}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5500" windowWidth="28040" windowHeight="17360" xr2:uid="{81856F94-4AA5-9242-8844-8A35083C4919}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>cc</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>random_field</t>
+  </si>
+  <si>
+    <t>country</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,24 +440,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>400000</v>
@@ -471,10 +471,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>600000</v>
@@ -488,10 +488,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>2000000</v>
@@ -513,10 +513,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
         <v>2500000</v>

</xml_diff>